<commit_message>
add info into form
</commit_message>
<xml_diff>
--- a/routes/Vòng1.xlsx
+++ b/routes/Vòng1.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:AI2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -419,56 +419,206 @@
         <v>Số điện thoại</v>
       </c>
       <c r="F1" t="str">
-        <v>Địa chỉ</v>
+        <v>Facebook</v>
       </c>
       <c r="G1" t="str">
-        <v>Nơi học/ làm việc</v>
+        <v>Trường đại học</v>
       </c>
       <c r="H1" t="str">
+        <v>Sinh viên</v>
+      </c>
+      <c r="I1" t="str">
         <v>Chuyên ngành</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" t="str">
+        <v>Thành tích, hoạt động nổi bật</v>
+      </c>
+      <c r="K1" t="str">
         <v>CV1</v>
       </c>
-      <c r="J1" t="str">
+      <c r="L1" t="str">
         <v>Có Team</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Tên nhóm</v>
+      </c>
+      <c r="N1" t="str">
+        <v>Họ và tên 2</v>
+      </c>
+      <c r="O1" t="str">
+        <v>Giới tính 2</v>
+      </c>
+      <c r="P1" t="str">
+        <v>Ngày sinh 2</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>Email 2</v>
+      </c>
+      <c r="R1" t="str">
+        <v>Số điện thoại 2</v>
+      </c>
+      <c r="S1" t="str">
+        <v>Facebook 2</v>
+      </c>
+      <c r="T1" t="str">
+        <v>Trường đại học 2</v>
+      </c>
+      <c r="U1" t="str">
+        <v>Sinh viên 2</v>
+      </c>
+      <c r="V1" t="str">
+        <v>Chuyên ngành 2</v>
+      </c>
+      <c r="W1" t="str">
+        <v>Thành tích, hoạt động nổi bật 2</v>
+      </c>
+      <c r="X1" t="str">
+        <v>CV2</v>
+      </c>
+      <c r="Y1" t="str">
+        <v>Họ và tên 3</v>
+      </c>
+      <c r="Z1" t="str">
+        <v>Giới tính 3</v>
+      </c>
+      <c r="AA1" t="str">
+        <v>Ngày sinh 3</v>
+      </c>
+      <c r="AB1" t="str">
+        <v>Email 3</v>
+      </c>
+      <c r="AC1" t="str">
+        <v>Số điện thoại 3</v>
+      </c>
+      <c r="AD1" t="str">
+        <v>Facebook 3</v>
+      </c>
+      <c r="AE1" t="str">
+        <v>Trường đại học 3</v>
+      </c>
+      <c r="AF1" t="str">
+        <v>Sinh viên 3</v>
+      </c>
+      <c r="AG1" t="str">
+        <v>Chuyên ngành 3</v>
+      </c>
+      <c r="AH1" t="str">
+        <v>Thành tích, hoạt động nổi bật 3</v>
+      </c>
+      <c r="AI1" t="str">
+        <v>CV3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Lê Công Bách</v>
+        <v>Sample</v>
       </c>
       <c r="B2" t="str">
-        <v>Nam</v>
+        <v>Khác</v>
       </c>
       <c r="C2" t="str">
-        <v>2022-04-21</v>
+        <v>2022-04-23</v>
       </c>
       <c r="D2" t="str">
-        <v>bachlamsung123@gmail.com</v>
+        <v>sample@email.com</v>
       </c>
       <c r="E2" t="str">
-        <v>0981583898</v>
+        <v>00000000000</v>
       </c>
       <c r="F2" t="str">
-        <v>Tổ 3, Phường Chiềng Lề</v>
+        <v>https://fb.com</v>
       </c>
       <c r="G2" t="str">
-        <v>fpt</v>
+        <v>Sample University</v>
       </c>
       <c r="H2" t="str">
-        <v>ktpm</v>
+        <v>Năm 1</v>
       </c>
       <c r="I2" t="str">
-        <v>uploads\1650543557765-475873022-Le-Cong-Bach-TopCV.vn-210422.163453.pdf</v>
+        <v>Sample Major</v>
       </c>
       <c r="J2" t="str">
-        <v>https://gecftu.com/manager/cv/uploads/Chưa</v>
+        <v>Sample Achievement</v>
+      </c>
+      <c r="K2" t="str">
+        <v>https://gecftu.com/manager/cv/uploads\1650701970888-104052759-SampleCV.pdf</v>
+      </c>
+      <c r="L2" t="str">
+        <v>Rồi</v>
+      </c>
+      <c r="M2" t="str">
+        <v>Sample Team</v>
+      </c>
+      <c r="N2" t="str">
+        <v>Sample 2</v>
+      </c>
+      <c r="O2" t="str">
+        <v>Khác</v>
+      </c>
+      <c r="P2" t="str">
+        <v>2022-04-23</v>
+      </c>
+      <c r="Q2" t="str">
+        <v>sample2@email.com</v>
+      </c>
+      <c r="R2" t="str">
+        <v>0000000000</v>
+      </c>
+      <c r="S2" t="str">
+        <v>https://www.fb.com</v>
+      </c>
+      <c r="T2" t="str">
+        <v>Sample University 2</v>
+      </c>
+      <c r="U2" t="str">
+        <v>Năm 2</v>
+      </c>
+      <c r="V2" t="str">
+        <v>Sample Major 2</v>
+      </c>
+      <c r="W2" t="str">
+        <v>Sample achievement</v>
+      </c>
+      <c r="X2" t="str">
+        <v>https://gecftu.com/manager/cv/uploads\1650702013769-603311779-SampleCV.pdf</v>
+      </c>
+      <c r="Y2" t="str">
+        <v>Sample 3</v>
+      </c>
+      <c r="Z2" t="str">
+        <v>Khác</v>
+      </c>
+      <c r="AA2" t="str">
+        <v>2022-04-23</v>
+      </c>
+      <c r="AB2" t="str">
+        <v>sample3@email.com</v>
+      </c>
+      <c r="AC2" t="str">
+        <v>0000000000</v>
+      </c>
+      <c r="AD2" t="str">
+        <v>https://fb.com/sample3</v>
+      </c>
+      <c r="AE2" t="str">
+        <v>Sample University 3</v>
+      </c>
+      <c r="AF2" t="str">
+        <v>Năm 3</v>
+      </c>
+      <c r="AG2" t="str">
+        <v>Sample Major 3</v>
+      </c>
+      <c r="AH2" t="str">
+        <v>Sample achievement</v>
+      </c>
+      <c r="AI2" t="str">
+        <v>https://gecftu.com/manager/cv/uploads\1650702013781-312483526-SampleCV.pdf</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AI2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>